<commit_message>
save before fight with unit tests
</commit_message>
<xml_diff>
--- a/src/main/resources/xlsx/limits.xlsx
+++ b/src/main/resources/xlsx/limits.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>11б</t>
   </si>
@@ -81,6 +81,12 @@
   </si>
   <si>
     <t>6в</t>
+  </si>
+  <si>
+    <t>Класс</t>
+  </si>
+  <si>
+    <t>Макс кол-во уроков</t>
   </si>
 </sst>
 </file>
@@ -433,25 +439,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1">
-        <v>5</v>
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -459,7 +465,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -467,7 +473,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -475,7 +481,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>5</v>
@@ -483,7 +489,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -491,15 +497,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -507,7 +513,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>6</v>
@@ -515,7 +521,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -523,7 +529,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
         <v>6</v>
@@ -531,7 +537,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
         <v>6</v>
@@ -539,15 +545,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -555,7 +561,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>7</v>
@@ -563,7 +569,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -571,7 +577,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -579,7 +585,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B18">
         <v>7</v>
@@ -587,9 +593,17 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B19">
+      <c r="B20">
         <v>7</v>
       </c>
     </row>

</xml_diff>